<commit_message>
Bug fixes and cleaning up
</commit_message>
<xml_diff>
--- a/data/portfolios/Yearly_portfolios.xlsx
+++ b/data/portfolios/Yearly_portfolios.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emil\Desktop\EPFL_python\FBD\project\data\portfolios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBBE949-BA28-4BE5-B50F-A74C57D329BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F1362D-96EC-4612-B6FA-949D25279188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{1F4FF791-28B5-4FE3-A400-89FDF0C5D683}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{1F4FF791-28B5-4FE3-A400-89FDF0C5D683}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Check of occurences" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Import data" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Sheet2!$A$1:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Check of occurences'!$D$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'Import data'!$A$1:$G$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="86">
   <si>
     <t># Stock</t>
   </si>
@@ -298,6 +300,12 @@
   </si>
   <si>
     <t>PROACT IT GROUP AB</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Nr of portfolios</t>
   </si>
 </sst>
 </file>
@@ -709,11 +717,1546 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0AAC7C8-1E41-46AA-98BD-AF791B495338}">
+  <dimension ref="A1:E121"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="45.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E33" si="0">COUNTIF($B$2:$B$121,D2)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34">
+        <f t="shared" ref="E34:E65" si="1">COUNTIF($B$2:$B$121,D34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>67</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" t="s">
+        <v>51</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>25</v>
+      </c>
+      <c r="D61" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" t="s">
+        <v>42</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D64" t="s">
+        <v>54</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" t="s">
+        <v>72</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66">
+        <f t="shared" ref="E66:E97" si="2">COUNTIF($B$2:$B$121,D66)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
+        <v>39</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>29</v>
+      </c>
+      <c r="D70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" t="s">
+        <v>77</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>75</v>
+      </c>
+      <c r="D76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>66</v>
+      </c>
+      <c r="D77" t="s">
+        <v>55</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="D1:E1" xr:uid="{854D0C25-0392-4EAA-9B40-226751C1292C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:E78">
+      <sortCondition descending="1" ref="E1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD94C4E3-BC4E-40C8-B9AF-32F118361511}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1681,11 +3224,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910B6D80-CCCF-4327-87EC-EE0520466734}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>